<commit_message>
Added link to spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Phase_4\Assignment_Phase_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A94E80E4-9513-40BE-9775-E6E03C06ECE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB8BA701-D1DB-404F-8A77-32D7BB189C73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5430" yWindow="2880" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>Assignment Name</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assingnment_2/UserAuthenticationTesting</t>
+  </si>
+  <si>
+    <t>Assignment 3</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_3/MovieAPI</t>
   </si>
 </sst>
 </file>
@@ -55,13 +61,6 @@
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -85,6 +84,14 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -134,25 +141,27 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -431,10 +440,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -474,12 +483,28 @@
         <v>6</v>
       </c>
       <c r="C3" s="2">
-        <v>45180</v>
+        <v>45181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="2">
+        <v>45182</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="B4" r:id="rId1" xr:uid="{00EB87AE-B345-446D-8720-78158FDF3338}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{EC5D0BD9-3AA5-44FE-A797-BC6CB860A5A1}"/>
+    <hyperlink ref="B2" r:id="rId3" xr:uid="{68559670-EA71-429B-96DE-7FB3587BB1B1}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Made changes in Spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Phase_4\Assignment_Phase_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68BC7040-7225-4EA4-B677-21BB58FB57CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30886C6E-8C89-4921-8918-3745DB17BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5025" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Assignment Name</t>
   </si>
@@ -64,6 +64,24 @@
   </si>
   <si>
     <t>D:\Training\Phase_4\Jenkins\MovieAPI\MovieAPI</t>
+  </si>
+  <si>
+    <t>Assignment 5</t>
+  </si>
+  <si>
+    <t>Assignment 6</t>
+  </si>
+  <si>
+    <t>Assignment 7</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_5/Calc</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_6</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_7</t>
   </si>
 </sst>
 </file>
@@ -137,7 +155,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -188,12 +206,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -211,6 +240,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -494,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,6 +605,39 @@
         <v>12</v>
       </c>
     </row>
+    <row r="6" spans="1:5" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="7">
+        <v>45184</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="7">
+        <v>45187</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="7">
+        <v>45188</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Changes made to spreadsheet
</commit_message>
<xml_diff>
--- a/Assignments.xlsx
+++ b/Assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training\Phase_4\Assignment_Phase_4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30886C6E-8C89-4921-8918-3745DB17BF56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B392882D-72E8-4D4E-A7E4-A52D87E964FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5025" yWindow="1710" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Assignment Name</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_7</t>
+  </si>
+  <si>
+    <t>Assignment 8</t>
+  </si>
+  <si>
+    <t>https://github.com/Vasanth30e/Assignment_Phase_4/tree/master/Assignment_8</t>
   </si>
 </sst>
 </file>
@@ -222,7 +228,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -247,6 +253,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -529,10 +538,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -638,6 +647,17 @@
         <v>45188</v>
       </c>
     </row>
+    <row r="9" spans="1:5" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="7">
+        <v>45189</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>

</xml_diff>